<commit_message>
finishes the first part of the second question
</commit_message>
<xml_diff>
--- a/Phase1-answer/Question1/Q2Data.xlsx
+++ b/Phase1-answer/Question1/Q2Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase1-answer\Question1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04A8AC4-56C0-410E-B966-382E2F5700DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C1A8BA-B760-4B62-836C-685F81CFE6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,11 +230,11 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,7 +749,7 @@
   <dimension ref="A3:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -804,7 +804,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -816,22 +816,22 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
         <v>200</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>487.96296296296288</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -842,7 +842,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -852,22 +852,22 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
         <v>512.03703703703707</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -878,7 +878,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -888,22 +888,22 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
         <v>57.500000000000114</v>
       </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
         <v>0</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -914,7 +914,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -924,27 +924,27 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
         <v>100</v>
       </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
         <v>675</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -954,22 +954,22 @@
       <c r="D8" s="1">
         <v>3</v>
       </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
         <v>367.49999999999989</v>
       </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="7">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1036,22 +1036,22 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>125.9259259259259</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>125.92592592592588</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>96.296296296296276</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>75.925925925925981</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>137.96296296296299</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>125.92592592592588</v>
       </c>
       <c r="L12" s="2" t="s">
@@ -1083,7 +1083,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1093,27 +1093,27 @@
       <c r="D13" s="1">
         <v>2</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>74.074074074074105</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>74.074074074074119</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>103.70370370370372</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>124.07407407407402</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>62.037037037037017</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <v>74.074074074074119</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1123,27 +1123,27 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
         <v>57.500000000000071</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1153,27 +1153,27 @@
       <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>200</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>200</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>100</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>50</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>25</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="6">
         <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1183,22 +1183,22 @@
       <c r="D16" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7">
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
         <v>100</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>150</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>117.49999999999993</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1232,7 +1232,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1244,27 +1244,27 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>374.07407407407413</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>248.14814814814827</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>151.85185185185196</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>75.925925925925981</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <v>137.96296296296299</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1274,27 +1274,27 @@
       <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>425.92592592592587</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>351.85185185185173</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>248.14814814814801</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>124.07407407407403</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>62.037037037037017</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1304,27 +1304,27 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>500</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>557.50000000000011</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>557.50000000000011</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="6">
         <v>557.50000000000011</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="6">
         <v>500</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1334,27 +1334,27 @@
       <c r="D23" s="1">
         <v>2</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>300</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>200</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>100</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="6">
         <v>50</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <v>25</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1364,22 +1364,22 @@
       <c r="D24" s="1">
         <v>3</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>500</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>500</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>767.49999999999989</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <v>617.49999999999989</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <v>500</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="6">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debugs input variebles of first part. all the answers changed
</commit_message>
<xml_diff>
--- a/Phase1-answer/Question1/Q2Data.xlsx
+++ b/Phase1-answer/Question1/Q2Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase1-answer\Question1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C1A8BA-B760-4B62-836C-685F81CFE6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF7548D-833F-437E-8312-79B0E9B21C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Veg</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Inventory Unit Cost</t>
+  </si>
+  <si>
+    <t>vegrefinelimit</t>
+  </si>
+  <si>
+    <t>oilrefinelimit</t>
   </si>
 </sst>
 </file>
@@ -516,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -738,6 +744,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -749,7 +771,7 @@
   <dimension ref="A3:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -800,7 +822,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="5">
-        <v>360000</v>
+        <v>405000</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -829,16 +851,16 @@
         <v>0</v>
       </c>
       <c r="I4" s="6">
-        <v>200</v>
+        <v>199.99999999999994</v>
       </c>
       <c r="J4" s="6">
-        <v>487.96296296296288</v>
+        <v>532.63888888888891</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M4" s="5">
-        <v>219357.87037037036</v>
+        <v>246493.14236111112</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -868,13 +890,13 @@
         <v>0</v>
       </c>
       <c r="J5" s="6">
-        <v>512.03703703703707</v>
+        <v>467.36111111111114</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M5" s="5">
-        <v>54662.5</v>
+        <v>54119.531250000007</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -892,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>57.500000000000114</v>
+        <v>32.5</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -910,7 +932,7 @@
         <v>26</v>
       </c>
       <c r="M6" s="5">
-        <v>85979.629629629635</v>
+        <v>104387.32638888888</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -928,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <v>100</v>
+        <v>37.500000000000341</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -940,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="6">
-        <v>675</v>
+        <v>732.03125</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -961,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="6">
-        <v>367.49999999999989</v>
+        <v>697.96874999999977</v>
       </c>
       <c r="H8" s="6">
         <v>0</v>
@@ -1037,22 +1059,22 @@
         <v>1</v>
       </c>
       <c r="E12" s="6">
-        <v>125.9259259259259</v>
+        <v>159.25925925925921</v>
       </c>
       <c r="F12" s="6">
-        <v>125.92592592592588</v>
+        <v>127.77777777777777</v>
       </c>
       <c r="G12" s="6">
-        <v>96.296296296296276</v>
+        <v>106.48148148148151</v>
       </c>
       <c r="H12" s="6">
-        <v>75.925925925925981</v>
+        <v>53.240740740740755</v>
       </c>
       <c r="I12" s="6">
-        <v>137.96296296296299</v>
+        <v>126.62037037037035</v>
       </c>
       <c r="J12" s="6">
-        <v>125.92592592592588</v>
+        <v>159.25925925925921</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>3</v>
@@ -1071,7 +1093,7 @@
       </c>
       <c r="P12" s="1">
         <f>SUMPRODUCT(H12:H16, input!$J$3:$J$7)/ SUM(output!H12:H16)</f>
-        <v>5.9625000000000004</v>
+        <v>5.7444444444444445</v>
       </c>
       <c r="Q12" s="1">
         <f>SUMPRODUCT(I12:I16, input!$J$3:$J$7)/ SUM(output!I12:I16)</f>
@@ -1094,22 +1116,22 @@
         <v>2</v>
       </c>
       <c r="E13" s="6">
-        <v>74.074074074074105</v>
+        <v>40.74074074074079</v>
       </c>
       <c r="F13" s="6">
-        <v>74.074074074074119</v>
+        <v>72.222222222222229</v>
       </c>
       <c r="G13" s="6">
-        <v>103.70370370370372</v>
+        <v>93.518518518518491</v>
       </c>
       <c r="H13" s="6">
-        <v>124.07407407407402</v>
+        <v>146.75925925925924</v>
       </c>
       <c r="I13" s="6">
-        <v>62.037037037037017</v>
+        <v>73.379629629629648</v>
       </c>
       <c r="J13" s="6">
-        <v>74.074074074074119</v>
+        <v>40.74074074074079</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1136,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="6">
-        <v>57.500000000000071</v>
+        <v>32.5</v>
       </c>
       <c r="J14" s="6">
         <v>0</v>
@@ -1154,22 +1176,22 @@
         <v>2</v>
       </c>
       <c r="E15" s="6">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="F15" s="6">
-        <v>200</v>
+        <v>143.75000000000017</v>
       </c>
       <c r="G15" s="6">
-        <v>100</v>
+        <v>71.875000000000085</v>
       </c>
       <c r="H15" s="6">
-        <v>50</v>
+        <v>35.937500000000043</v>
       </c>
       <c r="I15" s="6">
-        <v>25</v>
+        <v>17.968750000000021</v>
       </c>
       <c r="J15" s="6">
-        <v>200</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1187,16 +1209,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="6">
-        <v>0</v>
+        <v>106.24999999999984</v>
       </c>
       <c r="G16" s="6">
-        <v>100</v>
+        <v>178.12499999999991</v>
       </c>
       <c r="H16" s="6">
-        <v>150</v>
+        <v>214.06249999999994</v>
       </c>
       <c r="I16" s="6">
-        <v>117.49999999999993</v>
+        <v>199.53124999999997</v>
       </c>
       <c r="J16" s="6">
         <v>0</v>
@@ -1245,19 +1267,19 @@
         <v>1</v>
       </c>
       <c r="E20" s="6">
-        <v>374.07407407407413</v>
+        <v>340.74074074074076</v>
       </c>
       <c r="F20" s="6">
-        <v>248.14814814814827</v>
+        <v>212.96296296296302</v>
       </c>
       <c r="G20" s="6">
-        <v>151.85185185185196</v>
+        <v>106.48148148148151</v>
       </c>
       <c r="H20" s="6">
-        <v>75.925925925925981</v>
+        <v>53.240740740740755</v>
       </c>
       <c r="I20" s="6">
-        <v>137.96296296296299</v>
+        <v>126.62037037037035</v>
       </c>
       <c r="J20" s="6">
         <v>500</v>
@@ -1275,19 +1297,19 @@
         <v>2</v>
       </c>
       <c r="E21" s="6">
-        <v>425.92592592592587</v>
+        <v>459.25925925925924</v>
       </c>
       <c r="F21" s="6">
-        <v>351.85185185185173</v>
+        <v>387.03703703703701</v>
       </c>
       <c r="G21" s="6">
-        <v>248.14814814814801</v>
+        <v>293.51851851851853</v>
       </c>
       <c r="H21" s="6">
-        <v>124.07407407407403</v>
+        <v>146.7592592592593</v>
       </c>
       <c r="I21" s="6">
-        <v>62.037037037037017</v>
+        <v>73.379629629629648</v>
       </c>
       <c r="J21" s="6">
         <v>500</v>
@@ -1308,13 +1330,13 @@
         <v>500</v>
       </c>
       <c r="F22" s="6">
-        <v>557.50000000000011</v>
+        <v>532.5</v>
       </c>
       <c r="G22" s="6">
-        <v>557.50000000000011</v>
+        <v>532.5</v>
       </c>
       <c r="H22" s="6">
-        <v>557.50000000000011</v>
+        <v>532.5</v>
       </c>
       <c r="I22" s="6">
         <v>500</v>
@@ -1335,19 +1357,19 @@
         <v>2</v>
       </c>
       <c r="E23" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="F23" s="6">
-        <v>200</v>
+        <v>143.75000000000017</v>
       </c>
       <c r="G23" s="6">
-        <v>100</v>
+        <v>71.875000000000085</v>
       </c>
       <c r="H23" s="6">
-        <v>50</v>
+        <v>35.937500000000043</v>
       </c>
       <c r="I23" s="6">
-        <v>25</v>
+        <v>17.968750000000021</v>
       </c>
       <c r="J23" s="6">
         <v>500</v>
@@ -1368,13 +1390,13 @@
         <v>500</v>
       </c>
       <c r="F24" s="6">
-        <v>500</v>
+        <v>393.75000000000017</v>
       </c>
       <c r="G24" s="6">
-        <v>767.49999999999989</v>
+        <v>913.59375</v>
       </c>
       <c r="H24" s="6">
-        <v>617.49999999999989</v>
+        <v>699.53125</v>
       </c>
       <c r="I24" s="6">
         <v>500</v>

</xml_diff>

<commit_message>
makes the report for phase 1 final
</commit_message>
<xml_diff>
--- a/Phase1-answer/Question1/Q2Data.xlsx
+++ b/Phase1-answer/Question1/Q2Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase1-answer\Question1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF7548D-833F-437E-8312-79B0E9B21C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73E28C3-8508-450D-B647-4084210BDE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -771,7 +771,7 @@
   <dimension ref="A3:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>